<commit_message>
update before sending to Christopher
</commit_message>
<xml_diff>
--- a/bioprojects/maternal_carpenterbees_PRJNA437497/SraRunTable.xlsx
+++ b/bioprojects/maternal_carpenterbees_PRJNA437497/SraRunTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/gitreps/invert_meth_and_transcription/bioprojects/maternal_carpenterbees_PRJNA437497/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130E85FA-3B9E-7140-A189-052952CE2E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18825B98-ED90-E94F-928F-205A1CB1ECBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="3900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8480" yWindow="1680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="maternal_honeybees_PRJNA437497_" sheetId="1" r:id="rId1"/>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,6 +1300,7 @@
     <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2509,7 +2510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C52D99-08AB-AC4F-AD12-0BCFFE7FC11D}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>